<commit_message>
Fix report to patient link via patient_id
</commit_message>
<xml_diff>
--- a/covid19-rdt/covid_rdt.xlsx
+++ b/covid19-rdt/covid_rdt.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="188">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t xml:space="preserve">Contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_id</t>
   </si>
   <si>
     <t xml:space="preserve">Name</t>
@@ -999,8 +1002,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N8" activeCellId="0" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1282,50 +1285,52 @@
       <c r="AMI7" s="0"/>
       <c r="AMJ7" s="0"/>
     </row>
-    <row r="8" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="8" t="s">
+      <c r="B8" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="8" t="s">
+      <c r="C8" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="0"/>
+      <c r="E8" s="0"/>
+      <c r="F8" s="0"/>
+      <c r="G8" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="9"/>
-      <c r="AMB8" s="0"/>
-      <c r="AMC8" s="0"/>
-      <c r="AMD8" s="0"/>
-      <c r="AME8" s="0"/>
-      <c r="AMF8" s="0"/>
-      <c r="AMG8" s="0"/>
-      <c r="AMH8" s="0"/>
-      <c r="AMI8" s="0"/>
-      <c r="AMJ8" s="0"/>
-    </row>
-    <row r="9" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H8" s="0"/>
+      <c r="I8" s="0"/>
+      <c r="J8" s="0"/>
+      <c r="K8" s="0"/>
+      <c r="L8" s="0"/>
+      <c r="M8" s="0"/>
+      <c r="N8" s="0"/>
+      <c r="O8" s="0"/>
+      <c r="P8" s="0"/>
+      <c r="Q8" s="0"/>
+      <c r="R8" s="0"/>
+      <c r="S8" s="0"/>
+      <c r="T8" s="0"/>
+      <c r="U8" s="0"/>
+      <c r="V8" s="0"/>
+      <c r="W8" s="0"/>
+      <c r="X8" s="0"/>
+      <c r="Y8" s="0"/>
+      <c r="Z8" s="0"/>
+      <c r="AA8" s="0"/>
+    </row>
+    <row r="9" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>36</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
@@ -1340,6 +1345,7 @@
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
+      <c r="O9" s="16"/>
       <c r="P9" s="9"/>
       <c r="AMB9" s="0"/>
       <c r="AMC9" s="0"/>
@@ -1356,10 +1362,10 @@
         <v>24</v>
       </c>
       <c r="B10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -1387,18 +1393,20 @@
     </row>
     <row r="11" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
-      <c r="G11" s="8"/>
+      <c r="G11" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="H11" s="8"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
@@ -1417,23 +1425,28 @@
       <c r="AMI11" s="0"/>
       <c r="AMJ11" s="0"/>
     </row>
-    <row r="12" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
+    <row r="12" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="P12" s="9"/>
       <c r="AMB12" s="0"/>
       <c r="AMC12" s="0"/>
       <c r="AMD12" s="0"/>
@@ -1471,38 +1484,23 @@
       <c r="AMI13" s="0"/>
       <c r="AMJ13" s="0"/>
     </row>
-    <row r="14" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="N14" s="19"/>
-      <c r="R14" s="17" t="s">
-        <v>23</v>
-      </c>
+    <row r="14" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
       <c r="AMB14" s="0"/>
       <c r="AMC14" s="0"/>
       <c r="AMD14" s="0"/>
@@ -1513,29 +1511,33 @@
       <c r="AMI14" s="0"/>
       <c r="AMJ14" s="0"/>
     </row>
-    <row r="15" s="17" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="18" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
+        <v>46</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>48</v>
+      </c>
       <c r="G15" s="19"/>
       <c r="H15" s="19"/>
       <c r="I15" s="19"/>
       <c r="J15" s="19"/>
       <c r="K15" s="18"/>
       <c r="L15" s="19"/>
-      <c r="M15" s="18" t="s">
-        <v>51</v>
+      <c r="M15" s="0" t="s">
+        <v>49</v>
       </c>
       <c r="N15" s="19"/>
       <c r="R15" s="17" t="s">
@@ -1551,17 +1553,19 @@
       <c r="AMI15" s="0"/>
       <c r="AMJ15" s="0"/>
     </row>
-    <row r="16" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" s="17" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="18" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="19"/>
+        <v>51</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>46</v>
+      </c>
       <c r="E16" s="19"/>
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
@@ -1570,8 +1574,8 @@
       <c r="J16" s="19"/>
       <c r="K16" s="18"/>
       <c r="L16" s="19"/>
-      <c r="M16" s="20" t="s">
-        <v>54</v>
+      <c r="M16" s="18" t="s">
+        <v>52</v>
       </c>
       <c r="N16" s="19"/>
       <c r="R16" s="17" t="s">
@@ -1588,41 +1592,31 @@
       <c r="AMJ16" s="0"/>
     </row>
     <row r="17" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="21" t="s">
+      <c r="A17" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="22"/>
-      <c r="R17" s="22" t="s">
+      <c r="N17" s="19"/>
+      <c r="R17" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="S17" s="22"/>
-      <c r="T17" s="22"/>
-      <c r="U17" s="22"/>
-      <c r="V17" s="22"/>
-      <c r="W17" s="22"/>
-      <c r="X17" s="22"/>
-      <c r="Y17" s="22"/>
       <c r="AMB17" s="0"/>
       <c r="AMC17" s="0"/>
       <c r="AMD17" s="0"/>
@@ -1634,19 +1628,41 @@
       <c r="AMJ17" s="0"/>
     </row>
     <row r="18" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="H18" s="24"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="S18" s="22"/>
+      <c r="T18" s="22"/>
+      <c r="U18" s="22"/>
+      <c r="V18" s="22"/>
+      <c r="W18" s="22"/>
+      <c r="X18" s="22"/>
+      <c r="Y18" s="22"/>
       <c r="AMB18" s="0"/>
       <c r="AMC18" s="0"/>
       <c r="AMD18" s="0"/>
@@ -1659,11 +1675,13 @@
     </row>
     <row r="19" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="23" t="s">
         <v>60</v>
-      </c>
-      <c r="B19" s="0"/>
-      <c r="C19" s="23" t="s">
-        <v>61</v>
       </c>
       <c r="D19" s="24"/>
       <c r="E19" s="24"/>
@@ -1680,11 +1698,13 @@
       <c r="AMJ19" s="0"/>
     </row>
     <row r="20" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="24"/>
-      <c r="C20" s="0"/>
+      <c r="A20" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="0"/>
+      <c r="C20" s="23" t="s">
+        <v>62</v>
+      </c>
       <c r="D20" s="24"/>
       <c r="E20" s="24"/>
       <c r="F20" s="24"/>
@@ -1699,35 +1719,16 @@
       <c r="AMI20" s="0"/>
       <c r="AMJ20" s="0"/>
     </row>
-    <row r="21" s="22" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="R21" s="22" t="s">
-        <v>23</v>
-      </c>
+    <row r="21" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="24"/>
+      <c r="C21" s="0"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="H21" s="24"/>
       <c r="AMB21" s="0"/>
       <c r="AMC21" s="0"/>
       <c r="AMD21" s="0"/>
@@ -1738,27 +1739,34 @@
       <c r="AMI21" s="0"/>
       <c r="AMJ21" s="0"/>
     </row>
-    <row r="22" s="17" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+    <row r="22" s="22" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B22" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="J22" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="K22" s="0" t="s">
-        <v>69</v>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="R22" s="22" t="s">
+        <v>23</v>
       </c>
       <c r="AMB22" s="0"/>
       <c r="AMC22" s="0"/>
@@ -1770,16 +1778,28 @@
       <c r="AMI22" s="0"/>
       <c r="AMJ22" s="0"/>
     </row>
-    <row r="23" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="24"/>
-      <c r="C23" s="0"/>
-      <c r="D23" s="24"/>
+    <row r="23" s="17" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>46</v>
+      </c>
       <c r="E23" s="24"/>
       <c r="F23" s="24"/>
       <c r="H23" s="24"/>
+      <c r="J23" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="K23" s="0" t="s">
+        <v>70</v>
+      </c>
       <c r="AMB23" s="0"/>
       <c r="AMC23" s="0"/>
       <c r="AMD23" s="0"/>
@@ -1790,36 +1810,16 @@
       <c r="AMI23" s="0"/>
       <c r="AMJ23" s="0"/>
     </row>
-    <row r="24" s="22" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B24" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
-      <c r="R24" s="22" t="s">
-        <v>23</v>
-      </c>
+    <row r="24" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="24"/>
+      <c r="C24" s="0"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="H24" s="24"/>
       <c r="AMB24" s="0"/>
       <c r="AMC24" s="0"/>
       <c r="AMD24" s="0"/>
@@ -1830,27 +1830,35 @@
       <c r="AMI24" s="0"/>
       <c r="AMJ24" s="0"/>
     </row>
-    <row r="25" s="17" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="23" t="s">
+    <row r="25" s="22" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="B25" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="D25" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="J25" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="K25" s="23" t="s">
-        <v>76</v>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="R25" s="22" t="s">
+        <v>23</v>
       </c>
       <c r="AMB25" s="0"/>
       <c r="AMC25" s="0"/>
@@ -1862,16 +1870,28 @@
       <c r="AMI25" s="0"/>
       <c r="AMJ25" s="0"/>
     </row>
-    <row r="26" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="H26" s="1"/>
+    <row r="26" s="17" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="J26" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="K26" s="23" t="s">
+        <v>77</v>
+      </c>
       <c r="AMB26" s="0"/>
       <c r="AMC26" s="0"/>
       <c r="AMD26" s="0"/>
@@ -1882,36 +1902,16 @@
       <c r="AMI26" s="0"/>
       <c r="AMJ26" s="0"/>
     </row>
-    <row r="27" s="22" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="7"/>
-      <c r="P27" s="7"/>
-      <c r="R27" s="22" t="s">
-        <v>23</v>
-      </c>
+    <row r="27" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="H27" s="1"/>
       <c r="AMB27" s="0"/>
       <c r="AMC27" s="0"/>
       <c r="AMD27" s="0"/>
@@ -1922,29 +1922,36 @@
       <c r="AMI27" s="0"/>
       <c r="AMJ27" s="0"/>
     </row>
-    <row r="28" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="23" t="s">
+    <row r="28" s="22" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="B28" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D28" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="J28" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="K28" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="O28" s="0"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="R28" s="22" t="s">
+        <v>23</v>
+      </c>
       <c r="AMB28" s="0"/>
       <c r="AMC28" s="0"/>
       <c r="AMD28" s="0"/>
@@ -1957,19 +1964,27 @@
     </row>
     <row r="29" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29" s="24"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="24"/>
+        <v>80</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>46</v>
+      </c>
       <c r="E29" s="24"/>
       <c r="F29" s="24"/>
       <c r="H29" s="24"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="23"/>
-      <c r="O29" s="17" t="s">
+      <c r="J29" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="K29" s="23" t="s">
         <v>84</v>
       </c>
+      <c r="O29" s="0"/>
       <c r="AMB29" s="0"/>
       <c r="AMC29" s="0"/>
       <c r="AMD29" s="0"/>
@@ -1980,16 +1995,21 @@
       <c r="AMI29" s="0"/>
       <c r="AMJ29" s="0"/>
     </row>
-    <row r="30" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="H30" s="1"/>
+    <row r="30" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="24"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="23"/>
+      <c r="O30" s="17" t="s">
+        <v>85</v>
+      </c>
       <c r="AMB30" s="0"/>
       <c r="AMC30" s="0"/>
       <c r="AMD30" s="0"/>
@@ -2001,21 +2021,15 @@
       <c r="AMJ30" s="0"/>
     </row>
     <row r="31" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C31" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="D31" s="7"/>
+      <c r="A31" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
-      <c r="H31" s="7" t="s">
-        <v>64</v>
-      </c>
+      <c r="H31" s="1"/>
       <c r="AMB31" s="0"/>
       <c r="AMC31" s="0"/>
       <c r="AMD31" s="0"/>
@@ -2027,19 +2041,20 @@
       <c r="AMJ31" s="0"/>
     </row>
     <row r="32" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" s="24"/>
-      <c r="C32" s="0" t="s">
+      <c r="A32" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="D32" s="24"/>
+      <c r="C32" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" s="7"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="O32" s="26" t="s">
-        <v>87</v>
+      <c r="H32" s="7" t="s">
+        <v>65</v>
       </c>
       <c r="AMB32" s="0"/>
       <c r="AMC32" s="0"/>
@@ -2052,19 +2067,19 @@
       <c r="AMJ32" s="0"/>
     </row>
     <row r="33" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B33" s="1"/>
+      <c r="A33" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" s="24"/>
       <c r="C33" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="D33" s="1"/>
+        <v>87</v>
+      </c>
+      <c r="D33" s="24"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="H33" s="1"/>
       <c r="O33" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AMB33" s="0"/>
       <c r="AMC33" s="0"/>
@@ -2078,18 +2093,18 @@
     </row>
     <row r="34" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="24" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="H34" s="1"/>
       <c r="O34" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AMB34" s="0"/>
       <c r="AMC34" s="0"/>
@@ -2102,15 +2117,20 @@
       <c r="AMJ34" s="0"/>
     </row>
     <row r="35" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="25" t="s">
-        <v>31</v>
+      <c r="A35" s="24" t="s">
+        <v>61</v>
       </c>
       <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
+      <c r="C35" s="0" t="s">
+        <v>91</v>
+      </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="H35" s="1"/>
+      <c r="O35" s="26" t="s">
+        <v>92</v>
+      </c>
       <c r="AMB35" s="0"/>
       <c r="AMC35" s="0"/>
       <c r="AMD35" s="0"/>
@@ -2122,46 +2142,15 @@
       <c r="AMJ35" s="0"/>
     </row>
     <row r="36" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B36" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="C36" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="H36" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="I36" s="21"/>
-      <c r="J36" s="21"/>
-      <c r="K36" s="21"/>
-      <c r="L36" s="21"/>
-      <c r="M36" s="21"/>
-      <c r="N36" s="21"/>
-      <c r="O36" s="21"/>
-      <c r="P36" s="21"/>
-      <c r="Q36" s="21"/>
-      <c r="R36" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="S36" s="21"/>
-      <c r="T36" s="21"/>
-      <c r="U36" s="21"/>
-      <c r="V36" s="21"/>
-      <c r="W36" s="21"/>
-      <c r="X36" s="21"/>
-      <c r="Y36" s="21"/>
-      <c r="Z36" s="21"/>
-      <c r="AA36" s="21"/>
-      <c r="AB36" s="21"/>
+      <c r="A36" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="H36" s="1"/>
       <c r="AMB36" s="0"/>
       <c r="AMC36" s="0"/>
       <c r="AMD36" s="0"/>
@@ -2172,57 +2161,78 @@
       <c r="AMI36" s="0"/>
       <c r="AMJ36" s="0"/>
     </row>
-    <row r="37" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B37" s="24" t="s">
+    <row r="37" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I37" s="21"/>
+      <c r="J37" s="21"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="21"/>
+      <c r="M37" s="21"/>
+      <c r="N37" s="21"/>
+      <c r="O37" s="21"/>
+      <c r="P37" s="21"/>
+      <c r="Q37" s="21"/>
+      <c r="R37" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="S37" s="21"/>
+      <c r="T37" s="21"/>
+      <c r="U37" s="21"/>
+      <c r="V37" s="21"/>
+      <c r="W37" s="21"/>
+      <c r="X37" s="21"/>
+      <c r="Y37" s="21"/>
+      <c r="Z37" s="21"/>
+      <c r="AA37" s="21"/>
+      <c r="AB37" s="21"/>
+      <c r="AMB37" s="0"/>
+      <c r="AMC37" s="0"/>
+      <c r="AMD37" s="0"/>
+      <c r="AME37" s="0"/>
+      <c r="AMF37" s="0"/>
+      <c r="AMG37" s="0"/>
+      <c r="AMH37" s="0"/>
+      <c r="AMI37" s="0"/>
+      <c r="AMJ37" s="0"/>
+    </row>
+    <row r="38" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="D37" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="23" t="s">
+      <c r="C38" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="H37" s="24"/>
-      <c r="I37" s="17" t="n">
+      <c r="D38" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="E38" s="24"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="H38" s="24"/>
+      <c r="I38" s="17" t="n">
         <v>900</v>
-      </c>
-      <c r="AMB37" s="23"/>
-      <c r="AMC37" s="23"/>
-      <c r="AMD37" s="23"/>
-      <c r="AME37" s="23"/>
-      <c r="AMF37" s="23"/>
-      <c r="AMG37" s="23"/>
-      <c r="AMH37" s="23"/>
-      <c r="AMI37" s="23"/>
-      <c r="AMJ37" s="23"/>
-    </row>
-    <row r="38" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="J38" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="K38" s="26" t="s">
-        <v>101</v>
       </c>
       <c r="AMB38" s="23"/>
       <c r="AMC38" s="23"/>
@@ -2235,108 +2245,101 @@
       <c r="AMJ38" s="23"/>
     </row>
     <row r="39" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
+      <c r="A39" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="H39" s="1"/>
-      <c r="AMB39" s="0"/>
-      <c r="AMC39" s="0"/>
-      <c r="AMD39" s="0"/>
-      <c r="AME39" s="0"/>
-      <c r="AMF39" s="0"/>
-      <c r="AMG39" s="0"/>
-      <c r="AMH39" s="0"/>
-      <c r="AMI39" s="0"/>
-      <c r="AMJ39" s="0"/>
-    </row>
-    <row r="40" s="22" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="21" t="s">
+      <c r="J39" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="K39" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="AMB39" s="23"/>
+      <c r="AMC39" s="23"/>
+      <c r="AMD39" s="23"/>
+      <c r="AME39" s="23"/>
+      <c r="AMF39" s="23"/>
+      <c r="AMG39" s="23"/>
+      <c r="AMH39" s="23"/>
+      <c r="AMI39" s="23"/>
+      <c r="AMJ39" s="23"/>
+    </row>
+    <row r="40" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="AMB40" s="0"/>
+      <c r="AMC40" s="0"/>
+      <c r="AMD40" s="0"/>
+      <c r="AME40" s="0"/>
+      <c r="AMF40" s="0"/>
+      <c r="AMG40" s="0"/>
+      <c r="AMH40" s="0"/>
+      <c r="AMI40" s="0"/>
+      <c r="AMJ40" s="0"/>
+    </row>
+    <row r="41" s="22" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B40" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="C40" s="21" t="s">
+      <c r="B41" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="21" t="s">
+      <c r="C41" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="H40" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="I40" s="7"/>
-      <c r="J40" s="7"/>
-      <c r="K40" s="7"/>
-      <c r="L40" s="7"/>
-      <c r="M40" s="7"/>
-      <c r="N40" s="7"/>
-      <c r="O40" s="7"/>
-      <c r="P40" s="7"/>
-      <c r="R40" s="22" t="s">
+      <c r="H41" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="7"/>
+      <c r="P41" s="7"/>
+      <c r="R41" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="AMB40" s="23"/>
-      <c r="AMC40" s="23"/>
-      <c r="AMD40" s="23"/>
-      <c r="AME40" s="23"/>
-      <c r="AMF40" s="23"/>
-      <c r="AMG40" s="23"/>
-      <c r="AMH40" s="23"/>
-      <c r="AMI40" s="23"/>
-      <c r="AMJ40" s="23"/>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B41" s="0"/>
-      <c r="C41" s="0"/>
-      <c r="D41" s="0"/>
-      <c r="E41" s="0"/>
-      <c r="F41" s="0"/>
-      <c r="G41" s="0"/>
-      <c r="H41" s="0"/>
-      <c r="I41" s="0"/>
-      <c r="J41" s="0"/>
-      <c r="K41" s="0"/>
-      <c r="L41" s="0"/>
-      <c r="M41" s="0"/>
-      <c r="N41" s="0"/>
-      <c r="O41" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="P41" s="0"/>
-      <c r="Q41" s="0"/>
-      <c r="R41" s="0"/>
-      <c r="S41" s="0"/>
-      <c r="T41" s="0"/>
-      <c r="U41" s="0"/>
-      <c r="V41" s="0"/>
-      <c r="W41" s="0"/>
-      <c r="X41" s="0"/>
-      <c r="Y41" s="0"/>
-      <c r="Z41" s="0"/>
-      <c r="AA41" s="0"/>
+      <c r="AMB41" s="23"/>
+      <c r="AMC41" s="23"/>
+      <c r="AMD41" s="23"/>
+      <c r="AME41" s="23"/>
+      <c r="AMF41" s="23"/>
+      <c r="AMG41" s="23"/>
+      <c r="AMH41" s="23"/>
+      <c r="AMI41" s="23"/>
+      <c r="AMJ41" s="23"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="B42" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>107</v>
-      </c>
+      <c r="A42" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42" s="0"/>
+      <c r="C42" s="0"/>
       <c r="D42" s="0"/>
       <c r="E42" s="0"/>
       <c r="F42" s="0"/>
@@ -2348,7 +2351,9 @@
       <c r="L42" s="0"/>
       <c r="M42" s="0"/>
       <c r="N42" s="0"/>
-      <c r="O42" s="0"/>
+      <c r="O42" s="0" t="s">
+        <v>105</v>
+      </c>
       <c r="P42" s="0"/>
       <c r="Q42" s="0"/>
       <c r="R42" s="0"/>
@@ -2362,87 +2367,90 @@
       <c r="Z42" s="0"/>
       <c r="AA42" s="0"/>
     </row>
-    <row r="43" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="25" t="s">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="D43" s="0"/>
+      <c r="E43" s="0"/>
+      <c r="F43" s="0"/>
+      <c r="G43" s="0"/>
+      <c r="H43" s="0"/>
+      <c r="I43" s="0"/>
+      <c r="J43" s="0"/>
+      <c r="K43" s="0"/>
+      <c r="L43" s="0"/>
+      <c r="M43" s="0"/>
+      <c r="N43" s="0"/>
+      <c r="O43" s="0"/>
+      <c r="P43" s="0"/>
+      <c r="Q43" s="0"/>
+      <c r="R43" s="0"/>
+      <c r="S43" s="0"/>
+      <c r="T43" s="0"/>
+      <c r="U43" s="0"/>
+      <c r="V43" s="0"/>
+      <c r="W43" s="0"/>
+      <c r="X43" s="0"/>
+      <c r="Y43" s="0"/>
+      <c r="Z43" s="0"/>
+      <c r="AA43" s="0"/>
+    </row>
+    <row r="44" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="AMB43" s="23"/>
-      <c r="AMC43" s="23"/>
-      <c r="AMD43" s="23"/>
-      <c r="AME43" s="23"/>
-      <c r="AMF43" s="23"/>
-      <c r="AMG43" s="23"/>
-      <c r="AMH43" s="23"/>
-      <c r="AMI43" s="23"/>
-      <c r="AMJ43" s="23"/>
-    </row>
-    <row r="44" s="22" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="21" t="s">
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="AMB44" s="23"/>
+      <c r="AMC44" s="23"/>
+      <c r="AMD44" s="23"/>
+      <c r="AME44" s="23"/>
+      <c r="AMF44" s="23"/>
+      <c r="AMG44" s="23"/>
+      <c r="AMH44" s="23"/>
+      <c r="AMI44" s="23"/>
+      <c r="AMJ44" s="23"/>
+    </row>
+    <row r="45" s="22" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B44" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="C44" s="21" t="s">
+      <c r="B45" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="21" t="s">
+      <c r="C45" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="H44" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="I44" s="7"/>
-      <c r="J44" s="7"/>
-      <c r="K44" s="7"/>
-      <c r="L44" s="7"/>
-      <c r="M44" s="7"/>
-      <c r="N44" s="7"/>
-      <c r="O44" s="7"/>
-      <c r="P44" s="7"/>
-      <c r="R44" s="22" t="s">
+      <c r="H45" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="7"/>
+      <c r="N45" s="7"/>
+      <c r="O45" s="7"/>
+      <c r="P45" s="7"/>
+      <c r="R45" s="22" t="s">
         <v>23</v>
-      </c>
-      <c r="AMB44" s="0"/>
-      <c r="AMC44" s="0"/>
-      <c r="AMD44" s="0"/>
-      <c r="AME44" s="0"/>
-      <c r="AMF44" s="0"/>
-      <c r="AMG44" s="0"/>
-      <c r="AMH44" s="0"/>
-      <c r="AMI44" s="0"/>
-      <c r="AMJ44" s="0"/>
-    </row>
-    <row r="45" s="17" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="B45" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="D45" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="H45" s="24"/>
-      <c r="J45" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="K45" s="23" t="s">
-        <v>114</v>
       </c>
       <c r="AMB45" s="0"/>
       <c r="AMC45" s="0"/>
@@ -2454,16 +2462,28 @@
       <c r="AMI45" s="0"/>
       <c r="AMJ45" s="0"/>
     </row>
-    <row r="46" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="H46" s="1"/>
+    <row r="46" s="17" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="B46" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="D46" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="E46" s="24"/>
+      <c r="F46" s="24"/>
+      <c r="H46" s="24"/>
+      <c r="J46" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="K46" s="23" t="s">
+        <v>115</v>
+      </c>
       <c r="AMB46" s="0"/>
       <c r="AMC46" s="0"/>
       <c r="AMD46" s="0"/>
@@ -2474,74 +2494,57 @@
       <c r="AMI46" s="0"/>
       <c r="AMJ46" s="0"/>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="21" t="s">
+    <row r="47" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="AMB47" s="0"/>
+      <c r="AMC47" s="0"/>
+      <c r="AMD47" s="0"/>
+      <c r="AME47" s="0"/>
+      <c r="AMF47" s="0"/>
+      <c r="AMG47" s="0"/>
+      <c r="AMH47" s="0"/>
+      <c r="AMI47" s="0"/>
+      <c r="AMJ47" s="0"/>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B47" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="C47" s="21" t="s">
+      <c r="B48" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="D47" s="7"/>
-      <c r="G47" s="21" t="s">
+      <c r="C48" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="D48" s="7"/>
+      <c r="G48" s="21" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="48" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B48" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="C48" s="27" t="s">
-        <v>118</v>
-      </c>
-      <c r="D48" s="0"/>
-      <c r="E48" s="0"/>
-      <c r="F48" s="0"/>
-      <c r="G48" s="0"/>
-      <c r="H48" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="I48" s="0"/>
-      <c r="J48" s="0"/>
-      <c r="K48" s="0"/>
-      <c r="L48" s="0"/>
-      <c r="M48" s="0"/>
-      <c r="N48" s="0"/>
-      <c r="O48" s="0"/>
-      <c r="P48" s="0"/>
-      <c r="Q48" s="0"/>
-      <c r="R48" s="0"/>
-      <c r="S48" s="0"/>
-      <c r="T48" s="0"/>
-      <c r="U48" s="0"/>
-      <c r="V48" s="0"/>
-      <c r="W48" s="0"/>
-      <c r="X48" s="0"/>
-      <c r="Y48" s="0"/>
-      <c r="Z48" s="0"/>
-      <c r="AA48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C49" s="27" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D49" s="0"/>
       <c r="E49" s="0"/>
       <c r="F49" s="0"/>
       <c r="G49" s="0"/>
       <c r="H49" s="0" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I49" s="0"/>
       <c r="J49" s="0"/>
@@ -2565,20 +2568,20 @@
     </row>
     <row r="50" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C50" s="27" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D50" s="0"/>
       <c r="E50" s="0"/>
       <c r="F50" s="0"/>
       <c r="G50" s="0"/>
       <c r="H50" s="0" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I50" s="0"/>
       <c r="J50" s="0"/>
@@ -2600,22 +2603,22 @@
       <c r="Z50" s="0"/>
       <c r="AA50" s="0"/>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="C51" s="0" t="s">
-        <v>127</v>
+        <v>124</v>
+      </c>
+      <c r="C51" s="27" t="s">
+        <v>125</v>
       </c>
       <c r="D51" s="0"/>
       <c r="E51" s="0"/>
       <c r="F51" s="0"/>
       <c r="G51" s="0"/>
       <c r="H51" s="0" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I51" s="0"/>
       <c r="J51" s="0"/>
@@ -2639,19 +2642,21 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D52" s="0"/>
       <c r="E52" s="0"/>
       <c r="F52" s="0"/>
       <c r="G52" s="0"/>
-      <c r="H52" s="0"/>
+      <c r="H52" s="0" t="s">
+        <v>129</v>
+      </c>
       <c r="I52" s="0"/>
       <c r="J52" s="0"/>
       <c r="K52" s="0"/>
@@ -2673,11 +2678,45 @@
       <c r="AA52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="25" t="s">
+      <c r="A53" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="D53" s="0"/>
+      <c r="E53" s="0"/>
+      <c r="F53" s="0"/>
+      <c r="G53" s="0"/>
+      <c r="H53" s="0"/>
+      <c r="I53" s="0"/>
+      <c r="J53" s="0"/>
+      <c r="K53" s="0"/>
+      <c r="L53" s="0"/>
+      <c r="M53" s="0"/>
+      <c r="N53" s="0"/>
+      <c r="O53" s="0"/>
+      <c r="P53" s="0"/>
+      <c r="Q53" s="0"/>
+      <c r="R53" s="0"/>
+      <c r="S53" s="0"/>
+      <c r="T53" s="0"/>
+      <c r="U53" s="0"/>
+      <c r="V53" s="0"/>
+      <c r="W53" s="0"/>
+      <c r="X53" s="0"/>
+      <c r="Y53" s="0"/>
+      <c r="Z53" s="0"/>
+      <c r="AA53" s="0"/>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="25" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2756,7 +2795,7 @@
   <sheetData>
     <row r="1" s="31" customFormat="true" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B1" s="30" t="s">
         <v>1</v>
@@ -2769,231 +2808,231 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="23" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="23" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="23" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="23" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="23" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="23" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="23" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="23" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3073,40 +3112,40 @@
   <sheetData>
     <row r="1" s="31" customFormat="true" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="32" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E1" s="32" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F1" s="32" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" s="29" customFormat="true" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C2" s="23" t="str">
         <f aca="true">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2020-03-22  18-38</v>
+        <v>2020-03-22  19-33</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F2" s="33"/>
     </row>

</xml_diff>